<commit_message>
updated figures, fixed error bars
</commit_message>
<xml_diff>
--- a/2019_5_31_import_to_R_DOTA_Tras_225227.xlsx
+++ b/2019_5_31_import_to_R_DOTA_Tras_225227.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Days" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16453,8 +16454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G85" sqref="G85"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18579,9 +18580,9 @@
       <c r="A67">
         <v>3.6772985453372064E-6</v>
       </c>
-      <c r="B67" s="1">
-        <f>$B$66</f>
-        <v>3.1169728572759868E-5</v>
+      <c r="B67" s="2">
+        <f>0.00000001</f>
+        <v>1E-8</v>
       </c>
       <c r="C67">
         <v>3.0424785583827258E-3</v>
@@ -18610,12 +18611,12 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f>$A$67</f>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B68" s="1">
-        <f t="shared" ref="B68:B82" si="0">$B$66</f>
-        <v>3.1169728572759868E-5</v>
+        <f>0.00000001</f>
+        <v>1E-8</v>
+      </c>
+      <c r="B68" s="2">
+        <f t="shared" ref="B68:B82" si="0">0.00000001</f>
+        <v>1E-8</v>
       </c>
       <c r="C68">
         <v>4.4894297687675519E-3</v>
@@ -18644,12 +18645,12 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f t="shared" ref="A69:A82" si="1">$A$67</f>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B69" s="1">
+        <f t="shared" ref="A69:A82" si="1">0.00000001</f>
+        <v>1E-8</v>
+      </c>
+      <c r="B69" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C69">
         <v>7.1278236431375867E-3</v>
@@ -18679,11 +18680,11 @@
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B70" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B70" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C70">
         <v>9.9140595417599574E-3</v>
@@ -18713,11 +18714,11 @@
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B71" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B71" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C71">
         <v>1.2758164711773613E-2</v>
@@ -18747,11 +18748,11 @@
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B72" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B72" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C72">
         <v>1.5622122541673431E-2</v>
@@ -18781,11 +18782,11 @@
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B73" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B73" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C73">
         <v>1.8490306662119593E-2</v>
@@ -18815,11 +18816,11 @@
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B74" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B74" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C74">
         <v>2.1356393266010687E-2</v>
@@ -18849,11 +18850,11 @@
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B75" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B75" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C75">
         <v>2.4217897254033217E-2</v>
@@ -18883,11 +18884,11 @@
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B76" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B76" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C76">
         <v>2.9923729560848378E-2</v>
@@ -18917,11 +18918,11 @@
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B77" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B77" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C77">
         <v>3.7304906470641004E-2</v>
@@ -18951,11 +18952,11 @@
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B78" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B78" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C78">
         <v>7.7987536753899245E-2</v>
@@ -18985,11 +18986,11 @@
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B79" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B79" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C79">
         <v>0.15558555032853438</v>
@@ -19019,11 +19020,11 @@
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B80" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B80" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C80">
         <v>0.29685248896807293</v>
@@ -19053,11 +19054,11 @@
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B81" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B81" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C81">
         <v>0.53166437007620704</v>
@@ -19087,11 +19088,11 @@
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="1"/>
-        <v>3.6772985453372064E-6</v>
-      </c>
-      <c r="B82" s="1">
+        <v>1E-8</v>
+      </c>
+      <c r="B82" s="2">
         <f t="shared" si="0"/>
-        <v>3.1169728572759868E-5</v>
+        <v>1E-8</v>
       </c>
       <c r="C82">
         <v>0.66717789968697772</v>
@@ -24405,7 +24406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>

</xml_diff>